<commit_message>
renamed file from DatabaseOperations to ExcelOperations
</commit_message>
<xml_diff>
--- a/library_verificaton/BB.xlsx
+++ b/library_verificaton/BB.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,9 +15,23 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>SPA</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,14 +60,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -343,36 +366,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1">
+        <v>43640.512414733799</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1258</v>
+      </c>
+      <c r="G3" s="2">
+        <v>43640.512440081016</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>125</v>
+      </c>
+      <c r="G4" s="3">
+        <v>43640.512455370372</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>158</v>
+      </c>
+      <c r="G5" s="4">
+        <v>43640.512481527781</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>